<commit_message>
Return to more informative column headers.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10307"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odando/Documents/Job/Statistics/Spines GLMM/20190128.results/consolidated_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odando/Documents/Develop/git/LAB-AID/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A48F298-21ED-4E4C-817F-4FC0DB8B7C30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D010CF8A-D9F4-B546-B777-5485EB533AB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10720" windowWidth="33600" windowHeight="10280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fmr1 CA1" sheetId="1" r:id="rId1"/>
@@ -27,76 +27,76 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="24">
   <si>
-    <t>WT</t>
-  </si>
-  <si>
     <t>Seaside</t>
-  </si>
-  <si>
-    <t>KO</t>
   </si>
   <si>
     <t>EOFX</t>
   </si>
   <si>
-    <t>experiment_date</t>
+    <t>Control</t>
   </si>
   <si>
-    <t>line_name</t>
+    <t>Knockout</t>
   </si>
   <si>
-    <t>litter</t>
+    <t>Rheobase</t>
   </si>
   <si>
-    <t>age</t>
+    <t>Resting.Membrane.Potential</t>
   </si>
   <si>
-    <t>genotype</t>
+    <t>Membrane.Time.Constant</t>
   </si>
   <si>
-    <t>animal</t>
+    <t>Input.Resistance</t>
   </si>
   <si>
-    <t>slice</t>
+    <t>Action.Potential.Threshold</t>
   </si>
   <si>
-    <t>cell</t>
+    <t>Action.Potential.Amplitude</t>
   </si>
   <si>
-    <t>vm</t>
+    <t>Action.Potential.Maximum.Rise.Rate</t>
   </si>
   <si>
-    <t>tau</t>
+    <t>Action.Potential.Maximum.Decay.Rate</t>
   </si>
   <si>
-    <t>rinput</t>
+    <t>Action.Potential.Rise.Decay.Ratio</t>
   </si>
   <si>
-    <t>rheobase</t>
+    <t>Voltage.Sag</t>
   </si>
   <si>
-    <t>vthresh</t>
+    <t>Rebound.Slope</t>
   </si>
   <si>
-    <t>ap_ampl</t>
+    <t>Input.Resistance.From.Slope</t>
   </si>
   <si>
-    <t>ap_max_rise_rate</t>
+    <t>Experiment.Date</t>
   </si>
   <si>
-    <t>ap_max_decay_rate</t>
+    <t>Line.Name</t>
   </si>
   <si>
-    <t>rise_decay_ratio</t>
+    <t>Litter</t>
   </si>
   <si>
-    <t>sag</t>
+    <t>Age</t>
   </si>
   <si>
-    <t>rebound_slope</t>
+    <t>Genotype</t>
   </si>
   <si>
-    <t>rinput_slope</t>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Slice</t>
+  </si>
+  <si>
+    <t>Cell</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,64 +615,64 @@
   <sheetData>
     <row r="1" spans="1:35 16383:16383" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="R1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="S1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="T1" s="28" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:35 16383:16383" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>20160128</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="33">
         <v>20160118</v>
@@ -689,7 +689,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -748,7 +748,7 @@
         <v>20160128</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="33">
         <v>20160118</v>
@@ -757,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -825,7 +825,7 @@
         <v>20160128</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="33">
         <v>20160118</v>
@@ -834,7 +834,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -902,7 +902,7 @@
         <v>20160128</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="33">
         <v>20160118</v>
@@ -911,7 +911,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -979,7 +979,7 @@
         <v>20160128</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>20160118</v>
@@ -988,7 +988,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4">
         <v>2</v>
@@ -1056,7 +1056,7 @@
         <v>20160128</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>20160118</v>
@@ -1065,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -1133,7 +1133,7 @@
         <v>20160128</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>20160118</v>
@@ -1142,7 +1142,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -1195,7 +1195,7 @@
         <v>20160204</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>20160125</v>
@@ -1204,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -1257,7 +1257,7 @@
         <v>20160204</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>20160125</v>
@@ -1266,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -1319,7 +1319,7 @@
         <v>20160204</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>20160125</v>
@@ -1328,7 +1328,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1381,7 +1381,7 @@
         <v>20160204</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>20160125</v>
@@ -1390,7 +1390,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -1443,7 +1443,7 @@
         <v>20160204</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>20160125</v>
@@ -1452,7 +1452,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -1505,7 +1505,7 @@
         <v>20160204</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>20160125</v>
@@ -1514,7 +1514,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -1567,7 +1567,7 @@
         <v>20151214</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="31">
         <v>20151203</v>
@@ -1576,7 +1576,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
@@ -1629,7 +1629,7 @@
         <v>20151214</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="31">
         <v>20151203</v>
@@ -1638,7 +1638,7 @@
         <v>11</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -1691,7 +1691,7 @@
         <v>20151214</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="31">
         <v>20151203</v>
@@ -1700,7 +1700,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4">
         <v>2</v>
@@ -1753,7 +1753,7 @@
         <v>20151214</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="31">
         <v>20151203</v>
@@ -1762,7 +1762,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="4">
         <v>2</v>
@@ -1812,7 +1812,7 @@
         <v>20151214</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="31">
         <v>20151203</v>
@@ -1821,7 +1821,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -1874,7 +1874,7 @@
         <v>20151214</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="31">
         <v>20151203</v>
@@ -1883,7 +1883,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
@@ -1936,7 +1936,7 @@
         <v>20151214</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="31">
         <v>20151203</v>
@@ -1945,7 +1945,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="4">
         <v>2</v>
@@ -1998,7 +1998,7 @@
         <v>20160107</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="32">
         <v>20151227</v>
@@ -2007,7 +2007,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -2060,7 +2060,7 @@
         <v>20160107</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="32">
         <v>20151227</v>
@@ -2069,7 +2069,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -2137,7 +2137,7 @@
         <v>20160107</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="32">
         <v>20151227</v>
@@ -2146,7 +2146,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -2214,7 +2214,7 @@
         <v>20160107</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="32">
         <v>20151227</v>
@@ -2223,7 +2223,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
@@ -2291,7 +2291,7 @@
         <v>20160107</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="32">
         <v>20151227</v>
@@ -2300,7 +2300,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -2353,7 +2353,7 @@
         <v>20160107</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="32">
         <v>20151227</v>
@@ -2362,7 +2362,7 @@
         <v>11</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" s="4">
         <v>1</v>
@@ -2415,7 +2415,7 @@
         <v>20160107</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="32">
         <v>20151227</v>
@@ -2424,7 +2424,7 @@
         <v>11</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="4">
         <v>2</v>
@@ -2492,7 +2492,7 @@
         <v>20160107</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="32">
         <v>20151227</v>
@@ -2501,7 +2501,7 @@
         <v>11</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" s="4">
         <v>2</v>
@@ -2569,7 +2569,7 @@
         <v>20160107</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="32">
         <v>20151227</v>
@@ -2578,7 +2578,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" s="4">
         <v>2</v>
@@ -2646,7 +2646,7 @@
         <v>20160107</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="32">
         <v>20151227</v>
@@ -2655,7 +2655,7 @@
         <v>11</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" s="4">
         <v>2</v>
@@ -2723,7 +2723,7 @@
         <v>20160107</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="32">
         <v>20151227</v>
@@ -2732,7 +2732,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" s="4">
         <v>2</v>
@@ -2800,7 +2800,7 @@
         <v>20160107</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="32">
         <v>20151227</v>
@@ -2809,7 +2809,7 @@
         <v>11</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="4">
         <v>2</v>
@@ -2877,7 +2877,7 @@
         <v>20160107</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="32">
         <v>20151227</v>
@@ -2886,7 +2886,7 @@
         <v>11</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="4">
         <v>2</v>
@@ -2954,7 +2954,7 @@
         <v>20160205</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <v>20160125</v>
@@ -2963,7 +2963,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" s="4">
         <v>1</v>
@@ -3031,7 +3031,7 @@
         <v>20160205</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>20160125</v>
@@ -3040,7 +3040,7 @@
         <v>11</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="4">
         <v>1</v>
@@ -3108,7 +3108,7 @@
         <v>20160205</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>20160125</v>
@@ -3117,7 +3117,7 @@
         <v>11</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
@@ -3185,7 +3185,7 @@
         <v>20160205</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>20160125</v>
@@ -3194,7 +3194,7 @@
         <v>11</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="4">
         <v>1</v>
@@ -3247,7 +3247,7 @@
         <v>20160205</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>20160125</v>
@@ -3256,7 +3256,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" s="4">
         <v>2</v>
@@ -3309,7 +3309,7 @@
         <v>20160205</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>20160125</v>
@@ -3318,7 +3318,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="4">
         <v>2</v>
@@ -3371,7 +3371,7 @@
         <v>20160205</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>20160125</v>
@@ -3380,7 +3380,7 @@
         <v>11</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" s="4">
         <v>2</v>
@@ -3433,7 +3433,7 @@
         <v>20160205</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>20160125</v>
@@ -3442,7 +3442,7 @@
         <v>11</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" s="4">
         <v>2</v>
@@ -3495,7 +3495,7 @@
         <v>20160205</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>20160125</v>
@@ -3504,7 +3504,7 @@
         <v>11</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43" s="4">
         <v>2</v>
@@ -3557,7 +3557,7 @@
         <v>20160217</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44">
         <v>20160206</v>
@@ -3566,7 +3566,7 @@
         <v>11</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
@@ -3619,7 +3619,7 @@
         <v>20160217</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45">
         <v>20160206</v>
@@ -3628,7 +3628,7 @@
         <v>11</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" s="4">
         <v>1</v>
@@ -3683,7 +3683,7 @@
         <v>20160217</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>20160206</v>
@@ -3692,7 +3692,7 @@
         <v>11</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="4">
         <v>1</v>
@@ -3747,7 +3747,7 @@
         <v>20160217</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>20160206</v>
@@ -3756,7 +3756,7 @@
         <v>11</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="4">
         <v>1</v>
@@ -3811,7 +3811,7 @@
         <v>20160217</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>20160206</v>
@@ -3820,7 +3820,7 @@
         <v>11</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F48" s="4">
         <v>1</v>
@@ -3875,7 +3875,7 @@
         <v>20160217</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>20160206</v>
@@ -3884,7 +3884,7 @@
         <v>11</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49" s="4">
         <v>2</v>
@@ -3939,7 +3939,7 @@
         <v>20160217</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>20160206</v>
@@ -3948,7 +3948,7 @@
         <v>11</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F50" s="4">
         <v>2</v>
@@ -4001,7 +4001,7 @@
         <v>20160217</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51">
         <v>20160206</v>
@@ -4010,7 +4010,7 @@
         <v>11</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F51" s="4">
         <v>2</v>
@@ -4063,7 +4063,7 @@
         <v>20160217</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>20160206</v>
@@ -4072,7 +4072,7 @@
         <v>11</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F52" s="4">
         <v>2</v>
@@ -4125,7 +4125,7 @@
         <v>20160219</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53">
         <v>20160208</v>
@@ -4134,7 +4134,7 @@
         <v>11</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F53" s="4">
         <v>1</v>
@@ -4187,7 +4187,7 @@
         <v>20160219</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54">
         <v>20160208</v>
@@ -4196,7 +4196,7 @@
         <v>11</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F54" s="4">
         <v>1</v>
@@ -4249,7 +4249,7 @@
         <v>20160219</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
         <v>20160208</v>
@@ -4258,7 +4258,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F55" s="4">
         <v>1</v>
@@ -4311,7 +4311,7 @@
         <v>20160219</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56">
         <v>20160208</v>
@@ -4320,7 +4320,7 @@
         <v>11</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F56" s="4">
         <v>1</v>
@@ -4373,7 +4373,7 @@
         <v>20160219</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>20160208</v>
@@ -4382,7 +4382,7 @@
         <v>11</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F57" s="4">
         <v>1</v>
@@ -4435,7 +4435,7 @@
         <v>20160219</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>20160208</v>
@@ -4444,7 +4444,7 @@
         <v>11</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F58" s="4">
         <v>1</v>
@@ -4497,7 +4497,7 @@
         <v>20160219</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>20160208</v>
@@ -4506,7 +4506,7 @@
         <v>11</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F59" s="4">
         <v>2</v>
@@ -4559,7 +4559,7 @@
         <v>20160219</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60">
         <v>20160208</v>
@@ -4568,7 +4568,7 @@
         <v>11</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F60" s="4">
         <v>2</v>
@@ -4621,7 +4621,7 @@
         <v>20160219</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>20160208</v>
@@ -4630,7 +4630,7 @@
         <v>11</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F61" s="4">
         <v>2</v>
@@ -4685,7 +4685,7 @@
         <v>20160219</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>20160208</v>
@@ -4694,7 +4694,7 @@
         <v>11</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" s="4">
         <v>2</v>
@@ -4747,7 +4747,7 @@
         <v>20160219</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63">
         <v>20160208</v>
@@ -4756,7 +4756,7 @@
         <v>11</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="4">
         <v>2</v>
@@ -4809,7 +4809,7 @@
         <v>20160219</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64">
         <v>20160208</v>
@@ -4818,7 +4818,7 @@
         <v>11</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F64" s="4">
         <v>2</v>
@@ -4871,7 +4871,7 @@
         <v>20151216</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="18">
         <v>20151203</v>
@@ -4880,7 +4880,7 @@
         <v>12</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F65" s="6">
         <v>1</v>
@@ -4933,7 +4933,7 @@
         <v>20151216</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="18">
         <v>20151203</v>
@@ -4942,7 +4942,7 @@
         <v>12</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F66" s="6">
         <v>1</v>
@@ -4995,7 +4995,7 @@
         <v>20151216</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67" s="18">
         <v>20151203</v>
@@ -5004,7 +5004,7 @@
         <v>12</v>
       </c>
       <c r="E67" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F67" s="6">
         <v>1</v>
@@ -5057,7 +5057,7 @@
         <v>20151216</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68" s="18">
         <v>20151203</v>
@@ -5066,7 +5066,7 @@
         <v>12</v>
       </c>
       <c r="E68" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F68" s="6">
         <v>1</v>
@@ -5119,7 +5119,7 @@
         <v>20151216</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" s="18">
         <v>20151203</v>
@@ -5128,7 +5128,7 @@
         <v>12</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F69" s="6">
         <v>1</v>
@@ -5179,7 +5179,7 @@
         <v>20151216</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" s="18">
         <v>20151203</v>
@@ -5188,7 +5188,7 @@
         <v>12</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F70" s="6">
         <v>1</v>
@@ -5241,7 +5241,7 @@
         <v>20151216</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71" s="18">
         <v>20151203</v>
@@ -5250,7 +5250,7 @@
         <v>12</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F71" s="6">
         <v>1</v>
@@ -5303,7 +5303,7 @@
         <v>20151216</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72" s="18">
         <v>20151203</v>
@@ -5312,7 +5312,7 @@
         <v>12</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F72" s="6">
         <v>2</v>
@@ -5365,7 +5365,7 @@
         <v>20151216</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73" s="18">
         <v>20151203</v>
@@ -5374,7 +5374,7 @@
         <v>12</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F73" s="6">
         <v>2</v>
@@ -5427,7 +5427,7 @@
         <v>20151216</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C74" s="18">
         <v>20151203</v>
@@ -5436,7 +5436,7 @@
         <v>12</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74" s="6">
         <v>2</v>
@@ -5489,7 +5489,7 @@
         <v>20151216</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" s="18">
         <v>20151203</v>
@@ -5498,7 +5498,7 @@
         <v>12</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F75" s="6">
         <v>2</v>
@@ -5549,7 +5549,7 @@
         <v>20151216</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" s="18">
         <v>20151203</v>
@@ -5558,7 +5558,7 @@
         <v>12</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F76" s="6">
         <v>2</v>
@@ -5611,7 +5611,7 @@
         <v>20151216</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="18">
         <v>20151203</v>
@@ -5620,7 +5620,7 @@
         <v>12</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F77" s="6">
         <v>2</v>
@@ -5673,7 +5673,7 @@
         <v>20151223</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" s="18">
         <v>20151211</v>
@@ -5682,7 +5682,7 @@
         <v>12</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F78" s="6">
         <v>1</v>
@@ -5735,7 +5735,7 @@
         <v>20151223</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79" s="18">
         <v>20151211</v>
@@ -5744,7 +5744,7 @@
         <v>12</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79" s="6">
         <v>1</v>
@@ -5797,7 +5797,7 @@
         <v>20151223</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" s="18">
         <v>20151211</v>
@@ -5806,7 +5806,7 @@
         <v>12</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F80" s="6">
         <v>1</v>
@@ -5859,7 +5859,7 @@
         <v>20151223</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" s="18">
         <v>20151211</v>
@@ -5868,7 +5868,7 @@
         <v>12</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F81" s="6">
         <v>1</v>
@@ -5921,7 +5921,7 @@
         <v>20151223</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" s="18">
         <v>20151211</v>
@@ -5930,7 +5930,7 @@
         <v>12</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F82" s="6">
         <v>1</v>
@@ -5983,7 +5983,7 @@
         <v>20151223</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83" s="18">
         <v>20151211</v>
@@ -5992,7 +5992,7 @@
         <v>12</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F83" s="6">
         <v>1</v>
@@ -6045,7 +6045,7 @@
         <v>20151223</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" s="18">
         <v>20151211</v>
@@ -6054,7 +6054,7 @@
         <v>12</v>
       </c>
       <c r="E84" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F84" s="6">
         <v>3</v>
@@ -6107,7 +6107,7 @@
         <v>20151223</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" s="18">
         <v>20151211</v>
@@ -6116,7 +6116,7 @@
         <v>12</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F85" s="6">
         <v>3</v>
@@ -6169,7 +6169,7 @@
         <v>20151223</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" s="18">
         <v>20151211</v>
@@ -6178,7 +6178,7 @@
         <v>12</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F86" s="6">
         <v>3</v>
@@ -6231,7 +6231,7 @@
         <v>20160108</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" s="18">
         <v>20151227</v>
@@ -6240,7 +6240,7 @@
         <v>12</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87" s="6">
         <v>1</v>
@@ -6293,7 +6293,7 @@
         <v>20160108</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" s="18">
         <v>20151227</v>
@@ -6302,7 +6302,7 @@
         <v>12</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F88" s="6">
         <v>1</v>
@@ -6355,7 +6355,7 @@
         <v>20160108</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" s="18">
         <v>20151227</v>
@@ -6364,7 +6364,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F89" s="6">
         <v>1</v>
@@ -6417,7 +6417,7 @@
         <v>20160108</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" s="18">
         <v>20151227</v>
@@ -6426,7 +6426,7 @@
         <v>12</v>
       </c>
       <c r="E90" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F90" s="6">
         <v>1</v>
@@ -6479,7 +6479,7 @@
         <v>20160108</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91" s="18">
         <v>20151227</v>
@@ -6488,7 +6488,7 @@
         <v>12</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F91" s="6">
         <v>1</v>
@@ -6541,7 +6541,7 @@
         <v>20160108</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" s="18">
         <v>20151227</v>
@@ -6550,7 +6550,7 @@
         <v>12</v>
       </c>
       <c r="E92" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F92" s="6">
         <v>1</v>
@@ -6603,7 +6603,7 @@
         <v>20160108</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93" s="18">
         <v>20151227</v>
@@ -6612,7 +6612,7 @@
         <v>12</v>
       </c>
       <c r="E93" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F93" s="6">
         <v>1</v>
@@ -6665,7 +6665,7 @@
         <v>20160108</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" s="18">
         <v>20151227</v>
@@ -6674,7 +6674,7 @@
         <v>12</v>
       </c>
       <c r="E94" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F94" s="6">
         <v>1</v>
@@ -6727,7 +6727,7 @@
         <v>20160108</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" s="18">
         <v>20151227</v>
@@ -6736,7 +6736,7 @@
         <v>12</v>
       </c>
       <c r="E95" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F95" s="6">
         <v>1</v>
@@ -6789,7 +6789,7 @@
         <v>20160108</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96" s="18">
         <v>20151227</v>
@@ -6798,7 +6798,7 @@
         <v>12</v>
       </c>
       <c r="E96" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F96" s="6">
         <v>2</v>
@@ -6851,7 +6851,7 @@
         <v>20160108</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97" s="18">
         <v>20151227</v>
@@ -6860,7 +6860,7 @@
         <v>12</v>
       </c>
       <c r="E97" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F97" s="6">
         <v>2</v>
@@ -6913,7 +6913,7 @@
         <v>20160108</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" s="18">
         <v>20151227</v>
@@ -6922,7 +6922,7 @@
         <v>12</v>
       </c>
       <c r="E98" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F98" s="6">
         <v>2</v>
@@ -6975,7 +6975,7 @@
         <v>20160108</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" s="18">
         <v>20151227</v>
@@ -6984,7 +6984,7 @@
         <v>12</v>
       </c>
       <c r="E99" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F99" s="6">
         <v>2</v>
@@ -7037,7 +7037,7 @@
         <v>20160108</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" s="18">
         <v>20151227</v>
@@ -7046,7 +7046,7 @@
         <v>12</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F100" s="6">
         <v>2</v>
@@ -7099,7 +7099,7 @@
         <v>20160108</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="18">
         <v>20151227</v>
@@ -7108,7 +7108,7 @@
         <v>12</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F101" s="6">
         <v>2</v>
@@ -7161,7 +7161,7 @@
         <v>20160108</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102" s="18">
         <v>20151227</v>
@@ -7170,7 +7170,7 @@
         <v>12</v>
       </c>
       <c r="E102" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F102" s="6">
         <v>2</v>
@@ -7219,7 +7219,7 @@
         <v>20160108</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103" s="18">
         <v>20151227</v>
@@ -7228,7 +7228,7 @@
         <v>12</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F103" s="6">
         <v>2</v>
@@ -7281,7 +7281,7 @@
         <v>20160108</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104" s="18">
         <v>20151227</v>
@@ -7290,7 +7290,7 @@
         <v>12</v>
       </c>
       <c r="E104" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F104" s="6">
         <v>2</v>
@@ -7343,7 +7343,7 @@
         <v>20160108</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" s="18">
         <v>20151227</v>
@@ -7352,7 +7352,7 @@
         <v>12</v>
       </c>
       <c r="E105" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F105" s="6">
         <v>2</v>
@@ -7405,7 +7405,7 @@
         <v>20180124</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C106" s="18">
         <v>20180112</v>
@@ -7414,7 +7414,7 @@
         <v>12</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F106" s="6">
         <v>1</v>
@@ -7463,7 +7463,7 @@
         <v>20180124</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C107" s="18">
         <v>20180112</v>
@@ -7472,7 +7472,7 @@
         <v>12</v>
       </c>
       <c r="E107" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F107" s="6">
         <v>1</v>
@@ -7521,7 +7521,7 @@
         <v>20180209</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108" s="18">
         <v>20180128</v>
@@ -7530,7 +7530,7 @@
         <v>12</v>
       </c>
       <c r="E108" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F108" s="6">
         <v>2</v>
@@ -7579,7 +7579,7 @@
         <v>20160116</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109" s="18">
         <v>20160103</v>
@@ -7588,7 +7588,7 @@
         <v>13</v>
       </c>
       <c r="E109" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F109" s="6">
         <v>1</v>
@@ -7641,7 +7641,7 @@
         <v>20160116</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C110" s="18">
         <v>20160103</v>
@@ -7650,7 +7650,7 @@
         <v>13</v>
       </c>
       <c r="E110" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F110" s="6">
         <v>1</v>
@@ -7703,7 +7703,7 @@
         <v>20160116</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" s="18">
         <v>20160103</v>
@@ -7712,7 +7712,7 @@
         <v>13</v>
       </c>
       <c r="E111" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F111" s="6">
         <v>1</v>
@@ -7761,7 +7761,7 @@
         <v>20160116</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C112" s="18">
         <v>20160103</v>
@@ -7770,7 +7770,7 @@
         <v>13</v>
       </c>
       <c r="E112" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F112" s="6">
         <v>1</v>
@@ -7823,7 +7823,7 @@
         <v>20160116</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113" s="18">
         <v>20160103</v>
@@ -7832,7 +7832,7 @@
         <v>13</v>
       </c>
       <c r="E113" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F113" s="6">
         <v>1</v>
@@ -7885,7 +7885,7 @@
         <v>20160116</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" s="18">
         <v>20160103</v>
@@ -7894,7 +7894,7 @@
         <v>13</v>
       </c>
       <c r="E114" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F114" s="6">
         <v>1</v>
@@ -7947,7 +7947,7 @@
         <v>20160116</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C115" s="18">
         <v>20160103</v>
@@ -7956,7 +7956,7 @@
         <v>13</v>
       </c>
       <c r="E115" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F115" s="6">
         <v>1</v>
@@ -8009,7 +8009,7 @@
         <v>20160116</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C116" s="18">
         <v>20160103</v>
@@ -8018,7 +8018,7 @@
         <v>13</v>
       </c>
       <c r="E116" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F116" s="6">
         <v>1</v>
@@ -8071,7 +8071,7 @@
         <v>20160116</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" s="18">
         <v>20160103</v>
@@ -8080,7 +8080,7 @@
         <v>13</v>
       </c>
       <c r="E117" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F117" s="6">
         <v>1</v>
@@ -8133,7 +8133,7 @@
         <v>20180216</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C118" s="16">
         <v>20180203</v>
@@ -8142,7 +8142,7 @@
         <v>13</v>
       </c>
       <c r="E118" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F118" s="6">
         <v>1</v>
@@ -8191,7 +8191,7 @@
         <v>20150525</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C119" s="18">
         <v>20150511</v>
@@ -8200,7 +8200,7 @@
         <v>14</v>
       </c>
       <c r="E119" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F119" s="6">
         <v>1</v>
@@ -8253,7 +8253,7 @@
         <v>20150525</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C120" s="18">
         <v>20150511</v>
@@ -8262,7 +8262,7 @@
         <v>14</v>
       </c>
       <c r="E120" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F120" s="6">
         <v>1</v>
@@ -8315,7 +8315,7 @@
         <v>20150525</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121" s="18">
         <v>20150511</v>
@@ -8324,7 +8324,7 @@
         <v>14</v>
       </c>
       <c r="E121" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F121" s="6">
         <v>1</v>
@@ -8377,7 +8377,7 @@
         <v>20150525</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C122" s="18">
         <v>20150511</v>
@@ -8386,7 +8386,7 @@
         <v>14</v>
       </c>
       <c r="E122" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F122" s="6">
         <v>2</v>
@@ -8439,7 +8439,7 @@
         <v>20150525</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C123" s="18">
         <v>20150511</v>
@@ -8448,7 +8448,7 @@
         <v>14</v>
       </c>
       <c r="E123" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F123" s="6">
         <v>2</v>
@@ -8501,7 +8501,7 @@
         <v>20150810</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124" s="18">
         <v>20150727</v>
@@ -8510,7 +8510,7 @@
         <v>14</v>
       </c>
       <c r="E124" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F124" s="6">
         <v>1</v>
@@ -8563,7 +8563,7 @@
         <v>20150810</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C125" s="18">
         <v>20150727</v>
@@ -8572,7 +8572,7 @@
         <v>14</v>
       </c>
       <c r="E125" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F125" s="6">
         <v>1</v>
@@ -8625,7 +8625,7 @@
         <v>20150810</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C126" s="18">
         <v>20150727</v>
@@ -8634,7 +8634,7 @@
         <v>14</v>
       </c>
       <c r="E126" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F126" s="6">
         <v>1</v>
@@ -8687,7 +8687,7 @@
         <v>20150810</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C127" s="18">
         <v>20150727</v>
@@ -8696,7 +8696,7 @@
         <v>14</v>
       </c>
       <c r="E127" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F127" s="6">
         <v>1</v>
@@ -8749,7 +8749,7 @@
         <v>20150810</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C128" s="18">
         <v>20150727</v>
@@ -8758,7 +8758,7 @@
         <v>14</v>
       </c>
       <c r="E128" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F128" s="6">
         <v>1</v>
@@ -8811,7 +8811,7 @@
         <v>20150810</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C129" s="18">
         <v>20150727</v>
@@ -8820,7 +8820,7 @@
         <v>14</v>
       </c>
       <c r="E129" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F129" s="6">
         <v>1</v>
@@ -8873,7 +8873,7 @@
         <v>20151208</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C130" s="18">
         <v>20151124</v>
@@ -8882,7 +8882,7 @@
         <v>14</v>
       </c>
       <c r="E130" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F130" s="6">
         <v>1</v>
@@ -8933,7 +8933,7 @@
         <v>20151208</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" s="18">
         <v>20151124</v>
@@ -8942,7 +8942,7 @@
         <v>14</v>
       </c>
       <c r="E131" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F131" s="6">
         <v>1</v>
@@ -8995,7 +8995,7 @@
         <v>20160117</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C132" s="18">
         <v>20160103</v>
@@ -9004,7 +9004,7 @@
         <v>14</v>
       </c>
       <c r="E132" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F132" s="6">
         <v>1</v>
@@ -9057,7 +9057,7 @@
         <v>20160117</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C133" s="18">
         <v>20160103</v>
@@ -9066,7 +9066,7 @@
         <v>14</v>
       </c>
       <c r="E133" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F133" s="6">
         <v>1</v>
@@ -9119,7 +9119,7 @@
         <v>20160117</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C134" s="18">
         <v>20160103</v>
@@ -9128,7 +9128,7 @@
         <v>14</v>
       </c>
       <c r="E134" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F134" s="6">
         <v>1</v>
@@ -9181,7 +9181,7 @@
         <v>20160117</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C135" s="18">
         <v>20160103</v>
@@ -9190,7 +9190,7 @@
         <v>14</v>
       </c>
       <c r="E135" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F135" s="6">
         <v>1</v>
@@ -9243,7 +9243,7 @@
         <v>20160117</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C136" s="18">
         <v>20160103</v>
@@ -9252,7 +9252,7 @@
         <v>14</v>
       </c>
       <c r="E136" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F136" s="6">
         <v>1</v>
@@ -9305,7 +9305,7 @@
         <v>20160117</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137" s="18">
         <v>20160103</v>
@@ -9314,7 +9314,7 @@
         <v>14</v>
       </c>
       <c r="E137" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F137" s="6">
         <v>1</v>
@@ -9367,7 +9367,7 @@
         <v>20160117</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138" s="18">
         <v>20160103</v>
@@ -9376,7 +9376,7 @@
         <v>14</v>
       </c>
       <c r="E138" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F138" s="6">
         <v>1</v>
@@ -9429,7 +9429,7 @@
         <v>20160117</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C139" s="18">
         <v>20160103</v>
@@ -9438,7 +9438,7 @@
         <v>14</v>
       </c>
       <c r="E139" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F139" s="6">
         <v>1</v>
@@ -9491,7 +9491,7 @@
         <v>20180214</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C140" s="16">
         <v>20180201</v>
@@ -9500,7 +9500,7 @@
         <v>14</v>
       </c>
       <c r="E140" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F140" s="6">
         <v>1</v>
@@ -9549,7 +9549,7 @@
         <v>20150811</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C141" s="18">
         <v>20150727</v>
@@ -9558,7 +9558,7 @@
         <v>15</v>
       </c>
       <c r="E141" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F141" s="6">
         <v>2</v>
@@ -9611,7 +9611,7 @@
         <v>20150811</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C142" s="18">
         <v>20150727</v>
@@ -9620,7 +9620,7 @@
         <v>15</v>
       </c>
       <c r="E142" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F142" s="6">
         <v>2</v>
@@ -9673,7 +9673,7 @@
         <v>20150811</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C143" s="18">
         <v>20150727</v>
@@ -9682,7 +9682,7 @@
         <v>15</v>
       </c>
       <c r="E143" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F143" s="6">
         <v>2</v>
@@ -9735,7 +9735,7 @@
         <v>20150811</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C144" s="18">
         <v>20150727</v>
@@ -9744,7 +9744,7 @@
         <v>15</v>
       </c>
       <c r="E144" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F144" s="6">
         <v>2</v>
@@ -9797,7 +9797,7 @@
         <v>20150811</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C145" s="18">
         <v>20150727</v>
@@ -9806,7 +9806,7 @@
         <v>15</v>
       </c>
       <c r="E145" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F145" s="6">
         <v>2</v>
@@ -9859,7 +9859,7 @@
         <v>20150811</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C146" s="18">
         <v>20150727</v>
@@ -9868,7 +9868,7 @@
         <v>15</v>
       </c>
       <c r="E146" s="19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F146" s="6">
         <v>2</v>
@@ -9921,7 +9921,7 @@
         <v>20160204</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C147">
         <v>20160125</v>
@@ -9930,7 +9930,7 @@
         <v>10</v>
       </c>
       <c r="E147" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F147" s="4">
         <v>2</v>
@@ -9983,7 +9983,7 @@
         <v>20160204</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C148">
         <v>20160125</v>
@@ -9992,7 +9992,7 @@
         <v>10</v>
       </c>
       <c r="E148" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F148" s="4">
         <v>2</v>
@@ -10042,7 +10042,7 @@
         <v>20160204</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C149">
         <v>20160125</v>
@@ -10051,7 +10051,7 @@
         <v>10</v>
       </c>
       <c r="E149" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F149" s="4">
         <v>2</v>
@@ -10104,7 +10104,7 @@
         <v>20160204</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C150">
         <v>20160125</v>
@@ -10113,7 +10113,7 @@
         <v>10</v>
       </c>
       <c r="E150" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F150" s="4">
         <v>2</v>
@@ -10166,7 +10166,7 @@
         <v>20160204</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C151">
         <v>20160125</v>
@@ -10175,7 +10175,7 @@
         <v>10</v>
       </c>
       <c r="E151" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F151" s="4">
         <v>2</v>
@@ -10228,7 +10228,7 @@
         <v>20160204</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C152">
         <v>20160125</v>
@@ -10237,7 +10237,7 @@
         <v>10</v>
       </c>
       <c r="E152" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F152" s="4">
         <v>2</v>
@@ -10290,7 +10290,7 @@
         <v>20160218</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153">
         <v>20160208</v>
@@ -10299,7 +10299,7 @@
         <v>10</v>
       </c>
       <c r="E153" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F153" s="4">
         <v>1</v>
@@ -10349,7 +10349,7 @@
         <v>20160218</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C154">
         <v>20160208</v>
@@ -10358,7 +10358,7 @@
         <v>10</v>
       </c>
       <c r="E154" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F154" s="4">
         <v>1</v>
@@ -10411,7 +10411,7 @@
         <v>20160218</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C155">
         <v>20160208</v>
@@ -10420,7 +10420,7 @@
         <v>10</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F155" s="4">
         <v>1</v>
@@ -10473,7 +10473,7 @@
         <v>20160218</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C156">
         <v>20160208</v>
@@ -10482,7 +10482,7 @@
         <v>10</v>
       </c>
       <c r="E156" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F156" s="4">
         <v>1</v>
@@ -10535,7 +10535,7 @@
         <v>20160218</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C157">
         <v>20160208</v>
@@ -10544,7 +10544,7 @@
         <v>10</v>
       </c>
       <c r="E157" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F157" s="4">
         <v>1</v>
@@ -10594,7 +10594,7 @@
         <v>20160218</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C158">
         <v>20160208</v>
@@ -10603,7 +10603,7 @@
         <v>10</v>
       </c>
       <c r="E158" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F158" s="4">
         <v>2</v>
@@ -10656,7 +10656,7 @@
         <v>20160218</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159">
         <v>20160208</v>
@@ -10665,7 +10665,7 @@
         <v>10</v>
       </c>
       <c r="E159" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F159" s="4">
         <v>2</v>
@@ -10718,7 +10718,7 @@
         <v>20160218</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C160">
         <v>20160208</v>
@@ -10727,7 +10727,7 @@
         <v>10</v>
       </c>
       <c r="E160" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F160" s="4">
         <v>2</v>
@@ -10780,7 +10780,7 @@
         <v>20160218</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C161">
         <v>20160208</v>
@@ -10789,7 +10789,7 @@
         <v>10</v>
       </c>
       <c r="E161" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F161" s="4">
         <v>2</v>
@@ -10842,7 +10842,7 @@
         <v>20160218</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C162">
         <v>20160208</v>
@@ -10851,7 +10851,7 @@
         <v>10</v>
       </c>
       <c r="E162" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F162" s="4">
         <v>2</v>
@@ -10904,7 +10904,7 @@
         <v>20160220</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C163">
         <v>20160210</v>
@@ -10913,7 +10913,7 @@
         <v>10</v>
       </c>
       <c r="E163" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F163" s="4">
         <v>1</v>
@@ -10963,7 +10963,7 @@
         <v>20160220</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C164">
         <v>20160210</v>
@@ -10972,7 +10972,7 @@
         <v>10</v>
       </c>
       <c r="E164" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F164" s="4">
         <v>1</v>
@@ -11025,7 +11025,7 @@
         <v>20160220</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C165">
         <v>20160210</v>
@@ -11034,7 +11034,7 @@
         <v>10</v>
       </c>
       <c r="E165" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F165" s="4">
         <v>1</v>
@@ -11087,7 +11087,7 @@
         <v>20160220</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C166">
         <v>20160210</v>
@@ -11096,7 +11096,7 @@
         <v>10</v>
       </c>
       <c r="E166" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F166" s="4">
         <v>1</v>
@@ -11146,7 +11146,7 @@
         <v>20160220</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C167">
         <v>20160210</v>
@@ -11155,7 +11155,7 @@
         <v>10</v>
       </c>
       <c r="E167" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F167" s="4">
         <v>1</v>
@@ -11208,7 +11208,7 @@
         <v>20160220</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C168">
         <v>20160210</v>
@@ -11217,7 +11217,7 @@
         <v>10</v>
       </c>
       <c r="E168" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F168" s="4">
         <v>1</v>
@@ -11270,7 +11270,7 @@
         <v>20160220</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C169">
         <v>20160210</v>
@@ -11279,7 +11279,7 @@
         <v>10</v>
       </c>
       <c r="E169" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F169" s="4">
         <v>1</v>
@@ -11332,7 +11332,7 @@
         <v>20160220</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C170">
         <v>20160210</v>
@@ -11341,7 +11341,7 @@
         <v>10</v>
       </c>
       <c r="E170" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F170" s="4">
         <v>1</v>
@@ -11391,7 +11391,7 @@
         <v>20160220</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C171">
         <v>20160210</v>
@@ -11400,7 +11400,7 @@
         <v>10</v>
       </c>
       <c r="E171" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F171" s="4">
         <v>1</v>
@@ -11450,7 +11450,7 @@
         <v>20160220</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C172">
         <v>20160210</v>
@@ -11459,7 +11459,7 @@
         <v>10</v>
       </c>
       <c r="E172" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F172" s="4">
         <v>2</v>
@@ -11512,7 +11512,7 @@
         <v>20160220</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C173">
         <v>20160210</v>
@@ -11521,7 +11521,7 @@
         <v>10</v>
       </c>
       <c r="E173" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F173" s="4">
         <v>2</v>
@@ -11574,7 +11574,7 @@
         <v>20160220</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C174">
         <v>20160210</v>
@@ -11583,7 +11583,7 @@
         <v>10</v>
       </c>
       <c r="E174" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F174" s="4">
         <v>2</v>
@@ -11636,7 +11636,7 @@
         <v>20160220</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C175">
         <v>20160210</v>
@@ -11645,7 +11645,7 @@
         <v>10</v>
       </c>
       <c r="E175" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F175" s="4">
         <v>2</v>
@@ -11689,7 +11689,7 @@
         <v>20151214</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C176" s="31">
         <v>20151203</v>
@@ -11698,7 +11698,7 @@
         <v>11</v>
       </c>
       <c r="E176" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F176" s="4">
         <v>1</v>
@@ -11751,7 +11751,7 @@
         <v>20151214</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C177" s="31">
         <v>20151203</v>
@@ -11760,7 +11760,7 @@
         <v>11</v>
       </c>
       <c r="E177" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F177" s="4">
         <v>1</v>
@@ -11813,7 +11813,7 @@
         <v>20151215</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C178" s="18">
         <v>20151203</v>
@@ -11822,7 +11822,7 @@
         <v>12</v>
       </c>
       <c r="E178" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F178" s="6">
         <v>1</v>
@@ -11875,7 +11875,7 @@
         <v>20151215</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C179" s="18">
         <v>20151203</v>
@@ -11884,7 +11884,7 @@
         <v>12</v>
       </c>
       <c r="E179" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F179" s="6">
         <v>1</v>
@@ -11933,7 +11933,7 @@
         <v>20151215</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C180" s="18">
         <v>20151203</v>
@@ -11942,7 +11942,7 @@
         <v>12</v>
       </c>
       <c r="E180" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F180" s="6">
         <v>1</v>
@@ -11995,7 +11995,7 @@
         <v>20151215</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C181" s="18">
         <v>20151203</v>
@@ -12004,7 +12004,7 @@
         <v>12</v>
       </c>
       <c r="E181" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F181" s="6">
         <v>1</v>
@@ -12057,7 +12057,7 @@
         <v>20151215</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C182" s="18">
         <v>20151203</v>
@@ -12066,7 +12066,7 @@
         <v>12</v>
       </c>
       <c r="E182" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F182" s="6">
         <v>1</v>
@@ -12119,7 +12119,7 @@
         <v>20151215</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C183" s="18">
         <v>20151203</v>
@@ -12128,7 +12128,7 @@
         <v>12</v>
       </c>
       <c r="E183" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F183" s="6">
         <v>1</v>
@@ -12181,7 +12181,7 @@
         <v>20151215</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C184" s="18">
         <v>20151203</v>
@@ -12190,7 +12190,7 @@
         <v>12</v>
       </c>
       <c r="E184" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F184" s="6">
         <v>1</v>
@@ -12233,7 +12233,7 @@
         <v>20151215</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C185" s="18">
         <v>20151203</v>
@@ -12242,7 +12242,7 @@
         <v>12</v>
       </c>
       <c r="E185" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F185" s="6">
         <v>2</v>
@@ -12295,7 +12295,7 @@
         <v>20151215</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C186" s="18">
         <v>20151203</v>
@@ -12304,7 +12304,7 @@
         <v>12</v>
       </c>
       <c r="E186" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F186" s="6">
         <v>2</v>
@@ -12357,7 +12357,7 @@
         <v>20151215</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C187" s="18">
         <v>20151203</v>
@@ -12366,7 +12366,7 @@
         <v>12</v>
       </c>
       <c r="E187" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F187" s="6">
         <v>2</v>
@@ -12419,7 +12419,7 @@
         <v>20151215</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C188" s="18">
         <v>20151203</v>
@@ -12428,7 +12428,7 @@
         <v>12</v>
       </c>
       <c r="E188" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F188" s="6">
         <v>2</v>
@@ -12481,7 +12481,7 @@
         <v>20151223</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C189" s="18">
         <v>20151211</v>
@@ -12490,7 +12490,7 @@
         <v>12</v>
       </c>
       <c r="E189" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F189" s="6">
         <v>2</v>
@@ -12543,7 +12543,7 @@
         <v>20151223</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C190" s="18">
         <v>20151211</v>
@@ -12552,7 +12552,7 @@
         <v>12</v>
       </c>
       <c r="E190" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F190" s="6">
         <v>2</v>
@@ -12605,7 +12605,7 @@
         <v>20171218</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C191" s="16">
         <v>20171206</v>
@@ -12614,7 +12614,7 @@
         <v>12</v>
       </c>
       <c r="E191" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F191" s="4">
         <v>1</v>
@@ -12661,7 +12661,7 @@
         <v>20171218</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C192" s="16">
         <v>20171206</v>
@@ -12670,7 +12670,7 @@
         <v>12</v>
       </c>
       <c r="E192" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F192" s="4">
         <v>1</v>
@@ -12717,7 +12717,7 @@
         <v>20171218</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C193" s="16">
         <v>20171206</v>
@@ -12726,7 +12726,7 @@
         <v>12</v>
       </c>
       <c r="E193" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F193" s="6">
         <v>1</v>
@@ -12773,7 +12773,7 @@
         <v>20180124</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C194" s="18">
         <v>20180112</v>
@@ -12782,7 +12782,7 @@
         <v>12</v>
       </c>
       <c r="E194" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F194" s="4">
         <v>2</v>
@@ -12829,7 +12829,7 @@
         <v>20180124</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C195" s="18">
         <v>20180112</v>
@@ -12838,7 +12838,7 @@
         <v>12</v>
       </c>
       <c r="E195" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F195" s="4">
         <v>2</v>
@@ -12885,7 +12885,7 @@
         <v>20180124</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C196" s="18">
         <v>20180112</v>
@@ -12894,7 +12894,7 @@
         <v>12</v>
       </c>
       <c r="E196" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F196" s="4">
         <v>2</v>
@@ -12941,7 +12941,7 @@
         <v>20180209</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C197" s="18">
         <v>20180128</v>
@@ -12950,7 +12950,7 @@
         <v>12</v>
       </c>
       <c r="E197" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F197" s="4">
         <v>1</v>
@@ -12997,7 +12997,7 @@
         <v>20180209</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C198" s="18">
         <v>20180128</v>
@@ -13006,7 +13006,7 @@
         <v>12</v>
       </c>
       <c r="E198" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F198" s="4">
         <v>3</v>
@@ -13053,7 +13053,7 @@
         <v>20180212</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C199" s="16">
         <v>20180201</v>
@@ -13062,7 +13062,7 @@
         <v>12</v>
       </c>
       <c r="E199" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F199" s="4">
         <v>1</v>
@@ -13109,7 +13109,7 @@
         <v>20180215</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C200" s="16">
         <v>20180203</v>
@@ -13118,7 +13118,7 @@
         <v>12</v>
       </c>
       <c r="E200" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F200" s="4">
         <v>2</v>
@@ -13165,7 +13165,7 @@
         <v>20180215</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C201" s="16">
         <v>20180203</v>
@@ -13174,7 +13174,7 @@
         <v>12</v>
       </c>
       <c r="E201" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F201" s="4">
         <v>1</v>
@@ -13221,7 +13221,7 @@
         <v>20180215</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C202" s="16">
         <v>20180203</v>
@@ -13230,7 +13230,7 @@
         <v>12</v>
       </c>
       <c r="E202" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F202" s="4">
         <v>2</v>
@@ -13277,7 +13277,7 @@
         <v>20160116</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C203" s="18">
         <v>20160103</v>
@@ -13286,7 +13286,7 @@
         <v>13</v>
       </c>
       <c r="E203" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F203" s="6">
         <v>2</v>
@@ -13337,7 +13337,7 @@
         <v>20160116</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C204" s="18">
         <v>20160103</v>
@@ -13346,7 +13346,7 @@
         <v>13</v>
       </c>
       <c r="E204" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F204" s="6">
         <v>2</v>
@@ -13399,7 +13399,7 @@
         <v>20160116</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C205" s="18">
         <v>20160103</v>
@@ -13408,7 +13408,7 @@
         <v>13</v>
       </c>
       <c r="E205" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F205" s="6">
         <v>2</v>
@@ -13461,7 +13461,7 @@
         <v>20160116</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C206" s="18">
         <v>20160103</v>
@@ -13470,7 +13470,7 @@
         <v>13</v>
       </c>
       <c r="E206" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F206" s="6">
         <v>2</v>
@@ -13523,7 +13523,7 @@
         <v>20160116</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C207" s="18">
         <v>20160103</v>
@@ -13532,7 +13532,7 @@
         <v>13</v>
       </c>
       <c r="E207" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F207" s="6">
         <v>2</v>
@@ -13585,7 +13585,7 @@
         <v>20160116</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C208" s="18">
         <v>20160103</v>
@@ -13594,7 +13594,7 @@
         <v>13</v>
       </c>
       <c r="E208" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F208" s="6">
         <v>2</v>
@@ -13647,7 +13647,7 @@
         <v>20160116</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C209" s="18">
         <v>20160103</v>
@@ -13656,7 +13656,7 @@
         <v>13</v>
       </c>
       <c r="E209" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F209" s="6">
         <v>2</v>
@@ -13709,7 +13709,7 @@
         <v>20160116</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C210" s="18">
         <v>20160103</v>
@@ -13718,7 +13718,7 @@
         <v>13</v>
       </c>
       <c r="E210" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F210" s="6">
         <v>2</v>
@@ -13771,7 +13771,7 @@
         <v>20160116</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C211" s="18">
         <v>20160103</v>
@@ -13780,7 +13780,7 @@
         <v>13</v>
       </c>
       <c r="E211" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F211" s="6">
         <v>2</v>
@@ -13833,7 +13833,7 @@
         <v>20171219</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C212" s="16">
         <v>20171206</v>
@@ -13842,7 +13842,7 @@
         <v>13</v>
       </c>
       <c r="E212" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F212" s="4">
         <v>1</v>
@@ -13889,7 +13889,7 @@
         <v>20171219</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C213" s="16">
         <v>20171206</v>
@@ -13898,7 +13898,7 @@
         <v>13</v>
       </c>
       <c r="E213" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F213" s="4">
         <v>1</v>
@@ -13945,7 +13945,7 @@
         <v>20171219</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C214" s="16">
         <v>20171206</v>
@@ -13954,7 +13954,7 @@
         <v>13</v>
       </c>
       <c r="E214" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F214" s="4">
         <v>1</v>
@@ -14001,7 +14001,7 @@
         <v>20160117</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C215" s="18">
         <v>20160103</v>
@@ -14010,7 +14010,7 @@
         <v>14</v>
       </c>
       <c r="E215" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F215" s="6">
         <v>2</v>
@@ -14063,7 +14063,7 @@
         <v>20160117</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C216" s="18">
         <v>20160103</v>
@@ -14072,7 +14072,7 @@
         <v>14</v>
       </c>
       <c r="E216" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F216" s="6">
         <v>2</v>
@@ -14125,7 +14125,7 @@
         <v>20160117</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C217" s="18">
         <v>20160103</v>
@@ -14134,7 +14134,7 @@
         <v>14</v>
       </c>
       <c r="E217" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F217" s="6">
         <v>2</v>
@@ -14187,7 +14187,7 @@
         <v>20160117</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C218" s="18">
         <v>20160103</v>
@@ -14196,7 +14196,7 @@
         <v>14</v>
       </c>
       <c r="E218" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F218" s="6">
         <v>2</v>
@@ -14249,7 +14249,7 @@
         <v>20160117</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C219" s="18">
         <v>20160103</v>
@@ -14258,7 +14258,7 @@
         <v>14</v>
       </c>
       <c r="E219" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F219" s="6">
         <v>2</v>
@@ -14311,7 +14311,7 @@
         <v>20150811</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C220" s="18">
         <v>20150727</v>
@@ -14320,7 +14320,7 @@
         <v>15</v>
       </c>
       <c r="E220" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F220" s="6">
         <v>1</v>
@@ -14373,7 +14373,7 @@
         <v>20150811</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C221" s="18">
         <v>20150727</v>
@@ -14382,7 +14382,7 @@
         <v>15</v>
       </c>
       <c r="E221" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F221" s="6">
         <v>1</v>
@@ -14435,7 +14435,7 @@
         <v>20150811</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C222" s="18">
         <v>20150727</v>
@@ -14444,7 +14444,7 @@
         <v>15</v>
       </c>
       <c r="E222" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F222" s="6">
         <v>1</v>
@@ -14497,7 +14497,7 @@
         <v>20150811</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C223" s="18">
         <v>20150727</v>
@@ -14506,7 +14506,7 @@
         <v>15</v>
       </c>
       <c r="E223" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F223" s="6">
         <v>1</v>
@@ -14559,7 +14559,7 @@
         <v>20150811</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C224" s="18">
         <v>20150727</v>
@@ -14568,7 +14568,7 @@
         <v>15</v>
       </c>
       <c r="E224" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F224" s="6">
         <v>1</v>
@@ -14621,7 +14621,7 @@
         <v>20150811</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C225" s="18">
         <v>20150727</v>
@@ -14630,7 +14630,7 @@
         <v>15</v>
       </c>
       <c r="E225" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F225" s="6">
         <v>1</v>

</xml_diff>